<commit_message>
Ajout de la partie autoévaluation dans le rapport + le fichier PDF
</commit_message>
<xml_diff>
--- a/Doc/WIP/Journal-de-Travail_Lordon-Lucas - Copie.xlsx
+++ b/Doc/WIP/Journal-de-Travail_Lordon-Lucas - Copie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pu61qgw\Documents\GitHub\P_WEB295\Doc\WIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591DB095-29E5-40CC-916E-BF8A32AE7E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ACEB7AF-5D97-4E26-99A0-C86D279A48F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -119,9 +119,6 @@
     <t>Création du rapport selon le rapport</t>
   </si>
   <si>
-    <t>Discution avec AMG sur polygamie…</t>
-  </si>
-  <si>
     <t>Récupérer données de livres + Journal de travail</t>
   </si>
   <si>
@@ -204,6 +201,9 @@
   </si>
   <si>
     <t>C'est un enfer et cela ne fonctionne pas…</t>
+  </si>
+  <si>
+    <t>Discution avec AMG</t>
   </si>
 </sst>
 </file>
@@ -658,8 +658,8 @@
   <dimension ref="A1:N531"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -862,7 +862,7 @@
       </c>
       <c r="D11" s="11"/>
       <c r="E11" s="11" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="F11" s="11"/>
     </row>
@@ -880,7 +880,7 @@
         <v>8</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F12" s="11"/>
     </row>
@@ -898,10 +898,10 @@
         <v>7</v>
       </c>
       <c r="E13" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="11" t="s">
         <v>28</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -918,10 +918,10 @@
         <v>7</v>
       </c>
       <c r="E14" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="11" t="s">
         <v>30</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -938,10 +938,10 @@
         <v>11</v>
       </c>
       <c r="E15" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" s="11" t="s">
         <v>36</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -958,7 +958,7 @@
         <v>8</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F16" s="11"/>
     </row>
@@ -976,10 +976,10 @@
         <v>8</v>
       </c>
       <c r="E17" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="11" t="s">
         <v>39</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -996,7 +996,7 @@
         <v>8</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F18" s="11"/>
     </row>
@@ -1014,7 +1014,7 @@
         <v>8</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F19" s="11"/>
     </row>
@@ -1032,7 +1032,7 @@
         <v>8</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F20" s="11"/>
     </row>
@@ -1050,7 +1050,7 @@
         <v>8</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F21" s="11"/>
     </row>
@@ -1068,10 +1068,10 @@
         <v>8</v>
       </c>
       <c r="E22" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F22" s="11" t="s">
         <v>41</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1088,7 +1088,7 @@
         <v>8</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F23" s="11"/>
     </row>
@@ -1106,7 +1106,7 @@
         <v>8</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F24" s="11"/>
     </row>
@@ -1124,7 +1124,7 @@
         <v>8</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F25" s="11"/>
     </row>
@@ -1142,7 +1142,7 @@
         <v>8</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F26" s="11"/>
     </row>
@@ -1160,7 +1160,7 @@
         <v>11</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F27" s="11"/>
     </row>
@@ -1178,7 +1178,7 @@
         <v>8</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F28" s="11"/>
     </row>
@@ -1196,7 +1196,7 @@
         <v>8</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F29" s="11"/>
     </row>
@@ -1214,7 +1214,7 @@
         <v>8</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F30" s="11"/>
     </row>
@@ -1232,7 +1232,7 @@
         <v>8</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F31" s="11"/>
     </row>
@@ -1250,7 +1250,7 @@
         <v>8</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F32" s="11"/>
     </row>
@@ -1268,10 +1268,10 @@
         <v>8</v>
       </c>
       <c r="E33" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F33" s="11" t="s">
         <v>53</v>
-      </c>
-      <c r="F33" s="11" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -6785,26 +6785,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="83ae57d85107fc73e8c281aedb059e49">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b000e6a26fbebedf4c24f086a5622afe" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -7027,26 +7007,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{146BE2DA-6117-4657-9EA0-437EBB1E64B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7063,4 +7044,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>